<commit_message>
New version of Framework
</commit_message>
<xml_diff>
--- a/PageObjectwithFactories/src/test/resources/excel/testdata.xlsx
+++ b/PageObjectwithFactories/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\PageObjectwithFactories\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\git\PageObjectWithFactory\PageObjectwithFactories\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4288B1F9-6ED8-48D6-BAD9-314AB84A8A2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignInTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Y</t>
   </si>
@@ -73,15 +74,12 @@
   </si>
   <si>
     <t>noOfChildern</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -404,16 +402,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -424,7 +422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -432,10 +430,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -448,29 +446,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -493,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>